<commit_message>
kurthali sadak rebar size changed to 10mm and 3d dukha continued
</commit_message>
<xml_diff>
--- a/ofc/estimates/kurthali sadak/kurthali sadak.xlsx
+++ b/ofc/estimates/kurthali sadak/kurthali sadak.xlsx
@@ -839,17 +839,19 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -864,30 +866,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -907,6 +892,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1240,7 +1240,7 @@
       <sheetName val="PPMO_BOQ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="299">
           <cell r="B299" t="str">
@@ -1248,25 +1248,25 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1636,38 +1636,38 @@
       <c r="K5" s="119"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="120"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="112" t="s">
+      <c r="H6" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="113" t="s">
+      <c r="A7" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="113"/>
-      <c r="C7" s="113"/>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="113"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="112" t="s">
+      <c r="H7" s="121" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="121"/>
+      <c r="K7" s="121"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -3316,11 +3316,11 @@
       <c r="B73" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C73" s="114">
+      <c r="C73" s="112">
         <f>J71</f>
         <v>1194331.7948368895</v>
       </c>
-      <c r="D73" s="115"/>
+      <c r="D73" s="113"/>
       <c r="E73" s="16">
         <v>100</v>
       </c>
@@ -3335,21 +3335,21 @@
       <c r="B74" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C74" s="121">
+      <c r="C74" s="114">
         <v>1000000</v>
       </c>
-      <c r="D74" s="122"/>
+      <c r="D74" s="115"/>
       <c r="E74" s="16"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C75" s="121">
+      <c r="C75" s="114">
         <f>C74-C77-C78</f>
         <v>950000</v>
       </c>
-      <c r="D75" s="122"/>
+      <c r="D75" s="115"/>
       <c r="E75" s="16">
         <f>C75/C73*100</f>
         <v>79.542385466656867</v>
@@ -3359,11 +3359,11 @@
       <c r="B76" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="120">
+      <c r="C76" s="111">
         <f>C73-C75</f>
         <v>244331.79483688949</v>
       </c>
-      <c r="D76" s="120"/>
+      <c r="D76" s="111"/>
       <c r="E76" s="16">
         <f>100-E75</f>
         <v>20.457614533343133</v>
@@ -3373,11 +3373,11 @@
       <c r="B77" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C77" s="114">
+      <c r="C77" s="112">
         <f>C74*0.03</f>
         <v>30000</v>
       </c>
-      <c r="D77" s="115"/>
+      <c r="D77" s="113"/>
       <c r="E77" s="16">
         <v>3</v>
       </c>
@@ -3386,32 +3386,32 @@
       <c r="B78" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C78" s="114">
+      <c r="C78" s="112">
         <f>C74*0.02</f>
         <v>20000</v>
       </c>
-      <c r="D78" s="115"/>
+      <c r="D78" s="113"/>
       <c r="E78" s="16">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C76:D76"/>
     <mergeCell ref="C77:D77"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="C75:D75"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C73:D73"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3525,38 +3525,38 @@
       <c r="K5" s="119"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="120"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="112" t="s">
+      <c r="H6" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="113" t="s">
+      <c r="A7" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="113"/>
-      <c r="C7" s="113"/>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="113"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="112" t="s">
+      <c r="H7" s="121" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="121"/>
+      <c r="K7" s="121"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -4721,11 +4721,11 @@
       <c r="B55" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C55" s="114">
+      <c r="C55" s="112">
         <f>J53</f>
         <v>563311.92829411826</v>
       </c>
-      <c r="D55" s="115"/>
+      <c r="D55" s="113"/>
       <c r="E55" s="16">
         <v>100</v>
       </c>
@@ -4741,10 +4741,10 @@
       <c r="B56" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="121">
+      <c r="C56" s="114">
         <v>500000</v>
       </c>
-      <c r="D56" s="122"/>
+      <c r="D56" s="115"/>
       <c r="E56" s="16"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
@@ -4752,11 +4752,11 @@
       <c r="B57" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C57" s="121">
+      <c r="C57" s="114">
         <f>C56-C59-C60</f>
         <v>475000</v>
       </c>
-      <c r="D57" s="122"/>
+      <c r="D57" s="115"/>
       <c r="E57" s="16">
         <f>C57/C55*100</f>
         <v>84.322730647377924</v>
@@ -4767,11 +4767,11 @@
       <c r="B58" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C58" s="120">
+      <c r="C58" s="111">
         <f>C55-C57</f>
         <v>88311.928294118261</v>
       </c>
-      <c r="D58" s="120"/>
+      <c r="D58" s="111"/>
       <c r="E58" s="16">
         <f>100-E57</f>
         <v>15.677269352622076</v>
@@ -4782,11 +4782,11 @@
       <c r="B59" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C59" s="114">
+      <c r="C59" s="112">
         <f>C56*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D59" s="115"/>
+      <c r="D59" s="113"/>
       <c r="E59" s="16">
         <v>3</v>
       </c>
@@ -4796,24 +4796,17 @@
       <c r="B60" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C60" s="114">
+      <c r="C60" s="112">
         <f>C56*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D60" s="115"/>
+      <c r="D60" s="113"/>
       <c r="E60" s="16">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
     <mergeCell ref="A7:F7"/>
@@ -4822,6 +4815,13 @@
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="C58:D58"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4862,34 +4862,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="132" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="132"/>
+      <c r="J1" s="132"/>
+      <c r="K1" s="132"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
+      <c r="B2" s="133"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="133"/>
+      <c r="H2" s="133"/>
+      <c r="I2" s="133"/>
+      <c r="J2" s="133"/>
+      <c r="K2" s="133"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="118" t="s">
@@ -4922,30 +4922,30 @@
       <c r="K4" s="118"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="127" t="s">
+      <c r="A5" s="134" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="127"/>
-      <c r="C5" s="127"/>
-      <c r="D5" s="127"/>
-      <c r="E5" s="127"/>
-      <c r="F5" s="127"/>
-      <c r="G5" s="127"/>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="127"/>
-      <c r="K5" s="127"/>
+      <c r="B5" s="134"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="134"/>
     </row>
     <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="123" t="e">
+      <c r="C6" s="130" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="124"/>
+      <c r="D6" s="131"/>
       <c r="E6" s="13"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4953,11 +4953,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="12"/>
-      <c r="J6" s="123" t="e">
+      <c r="J6" s="130" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="124"/>
+      <c r="K6" s="131"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
@@ -4966,77 +4966,77 @@
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
-      <c r="F7" s="130"/>
-      <c r="G7" s="130"/>
-      <c r="I7" s="131" t="s">
+      <c r="F7" s="125"/>
+      <c r="G7" s="125"/>
+      <c r="I7" s="126" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="131"/>
-      <c r="K7" s="131"/>
+      <c r="J7" s="126"/>
+      <c r="K7" s="126"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="111" t="str">
+      <c r="A8" s="120" t="str">
         <f>Estimate!A6</f>
         <v>Project:- बेन्डोल हाईट सडक निर्माण</v>
       </c>
-      <c r="B8" s="111"/>
-      <c r="C8" s="111"/>
-      <c r="D8" s="111"/>
-      <c r="E8" s="111"/>
-      <c r="F8" s="111"/>
-      <c r="I8" s="132" t="s">
+      <c r="B8" s="120"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
+      <c r="I8" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="132"/>
-      <c r="K8" s="132"/>
+      <c r="J8" s="127"/>
+      <c r="K8" s="127"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="133" t="str">
+      <c r="A9" s="128" t="str">
         <f>Estimate!A7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="133"/>
-      <c r="C9" s="133"/>
-      <c r="D9" s="133"/>
-      <c r="E9" s="133"/>
-      <c r="F9" s="133"/>
-      <c r="I9" s="132" t="s">
+      <c r="B9" s="128"/>
+      <c r="C9" s="128"/>
+      <c r="D9" s="128"/>
+      <c r="E9" s="128"/>
+      <c r="F9" s="128"/>
+      <c r="I9" s="127" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="132"/>
-      <c r="K9" s="132"/>
+      <c r="J9" s="127"/>
+      <c r="K9" s="127"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="128" t="s">
+      <c r="A11" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="128" t="s">
+      <c r="B11" s="123" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="128" t="s">
+      <c r="C11" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="134" t="s">
+      <c r="D11" s="129" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="134"/>
-      <c r="F11" s="134"/>
-      <c r="G11" s="134" t="s">
+      <c r="E11" s="129"/>
+      <c r="F11" s="129"/>
+      <c r="G11" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="134"/>
-      <c r="I11" s="134"/>
-      <c r="J11" s="128" t="s">
+      <c r="H11" s="129"/>
+      <c r="I11" s="129"/>
+      <c r="J11" s="123" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="129" t="s">
+      <c r="K11" s="124" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="128"/>
-      <c r="B12" s="128"/>
-      <c r="C12" s="128"/>
+      <c r="A12" s="123"/>
+      <c r="B12" s="123"/>
+      <c r="C12" s="123"/>
       <c r="D12" s="15" t="s">
         <v>26</v>
       </c>
@@ -5055,8 +5055,8 @@
       <c r="I12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="128"/>
-      <c r="K12" s="129"/>
+      <c r="J12" s="123"/>
+      <c r="K12" s="124"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
@@ -5218,6 +5218,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -5231,13 +5238,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5349,21 +5349,21 @@
       <c r="K5" s="119"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="120" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="120"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="112" t="s">
+      <c r="H6" s="121" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="135" t="s">
@@ -6621,21 +6621,21 @@
       <c r="K5" s="119"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="120" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="120"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="112" t="s">
+      <c r="H6" s="121" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="135" t="s">
@@ -7920,13 +7920,6 @@
     <row r="112" s="75" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="C55:D55"/>
     <mergeCell ref="A7:F7"/>
@@ -7935,6 +7928,13 @@
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="C53:D53"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -8039,21 +8039,21 @@
       <c r="K5" s="119"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="120" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="120"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="112" t="s">
+      <c r="H6" s="121" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="135" t="s">
@@ -9370,6 +9370,13 @@
     <row r="113" s="75" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C55:D55"/>
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="A7:F7"/>
@@ -9378,13 +9385,6 @@
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="C54:D54"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -9395,8 +9395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9489,21 +9489,21 @@
       <c r="K5" s="119"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="120" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="120"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="112" t="s">
+      <c r="H6" s="121" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="135" t="s">
@@ -9592,7 +9592,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="78">
-        <v>12.5</v>
+        <v>12.15</v>
       </c>
       <c r="E10" s="78">
         <v>0.45</v>
@@ -9603,7 +9603,7 @@
       </c>
       <c r="G10" s="79">
         <f>PRODUCT(C10:F10)</f>
-        <v>9</v>
+        <v>8.7480000000000011</v>
       </c>
       <c r="H10" s="80"/>
       <c r="I10" s="80"/>
@@ -9626,8 +9626,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="78">
-        <f>D10</f>
-        <v>12.5</v>
+        <v>12.15</v>
       </c>
       <c r="E11" s="78">
         <v>4</v>
@@ -9637,7 +9636,7 @@
       </c>
       <c r="G11" s="79">
         <f>PRODUCT(C11:F11)</f>
-        <v>7.5</v>
+        <v>7.29</v>
       </c>
       <c r="H11" s="80"/>
       <c r="I11" s="80"/>
@@ -9662,7 +9661,7 @@
       <c r="F12" s="32"/>
       <c r="G12" s="34">
         <f>SUM(G10:G11)</f>
-        <v>16.5</v>
+        <v>16.038</v>
       </c>
       <c r="H12" s="33" t="s">
         <v>49</v>
@@ -9672,7 +9671,7 @@
       </c>
       <c r="J12" s="81">
         <f>G12*I12</f>
-        <v>1066.395</v>
+        <v>1036.53594</v>
       </c>
       <c r="K12" s="32"/>
       <c r="M12" s="36"/>
@@ -9697,7 +9696,7 @@
       <c r="I13" s="34"/>
       <c r="J13" s="81">
         <f>0.13*G12*19284/360</f>
-        <v>114.90049999999999</v>
+        <v>111.68328600000001</v>
       </c>
       <c r="K13" s="32"/>
       <c r="M13" s="36"/>
@@ -9762,7 +9761,7 @@
       </c>
       <c r="D16" s="78">
         <f>D11</f>
-        <v>12.5</v>
+        <v>12.15</v>
       </c>
       <c r="E16" s="78">
         <v>4</v>
@@ -9772,7 +9771,7 @@
       </c>
       <c r="G16" s="79">
         <f>PRODUCT(C16:F16)</f>
-        <v>15</v>
+        <v>14.58</v>
       </c>
       <c r="H16" s="80"/>
       <c r="I16" s="80"/>
@@ -9797,7 +9796,7 @@
       <c r="F17" s="32"/>
       <c r="G17" s="34">
         <f>SUM(G16:G16)</f>
-        <v>15</v>
+        <v>14.58</v>
       </c>
       <c r="H17" s="33" t="s">
         <v>49</v>
@@ -9807,7 +9806,7 @@
       </c>
       <c r="J17" s="81">
         <f>G17*I17</f>
-        <v>6064.2</v>
+        <v>5894.4023999999999</v>
       </c>
       <c r="K17" s="32"/>
       <c r="M17" s="36"/>
@@ -9874,7 +9873,7 @@
       </c>
       <c r="D20" s="78">
         <f>D16</f>
-        <v>12.5</v>
+        <v>12.15</v>
       </c>
       <c r="E20" s="78">
         <f>E11</f>
@@ -9885,7 +9884,7 @@
       </c>
       <c r="G20" s="79">
         <f>PRODUCT(C20:F20)</f>
-        <v>7.5</v>
+        <v>7.29</v>
       </c>
       <c r="H20" s="80"/>
       <c r="I20" s="80"/>
@@ -9910,7 +9909,7 @@
       <c r="F21" s="83"/>
       <c r="G21" s="53">
         <f>SUM(G20:G20)</f>
-        <v>7.5</v>
+        <v>7.29</v>
       </c>
       <c r="H21" s="53" t="s">
         <v>49</v>
@@ -9920,7 +9919,7 @@
       </c>
       <c r="J21" s="84">
         <f>G21*I21</f>
-        <v>34211.474999999999</v>
+        <v>33253.553699999997</v>
       </c>
       <c r="K21" s="76"/>
     </row>
@@ -9938,7 +9937,7 @@
       <c r="I22" s="83"/>
       <c r="J22" s="85">
         <f>0.13*G21*(15452.6/5)</f>
-        <v>3013.2570000000001</v>
+        <v>2928.885804</v>
       </c>
       <c r="K22" s="76"/>
     </row>
@@ -9991,7 +9990,7 @@
       </c>
       <c r="D25" s="78">
         <f>D10</f>
-        <v>12.5</v>
+        <v>12.15</v>
       </c>
       <c r="E25" s="78">
         <f>E10</f>
@@ -10002,7 +10001,7 @@
       </c>
       <c r="G25" s="79">
         <f>PRODUCT(C25:F25)</f>
-        <v>0.84375</v>
+        <v>0.82012499999999999</v>
       </c>
       <c r="H25" s="80"/>
       <c r="I25" s="80"/>
@@ -10027,7 +10026,7 @@
       <c r="F26" s="83"/>
       <c r="G26" s="53">
         <f>SUM(G25:G25)</f>
-        <v>0.84375</v>
+        <v>0.82012499999999999</v>
       </c>
       <c r="H26" s="53" t="s">
         <v>49</v>
@@ -10037,7 +10036,7 @@
       </c>
       <c r="J26" s="84">
         <f>G26*I26</f>
-        <v>8972.859375</v>
+        <v>8721.6193124999991</v>
       </c>
       <c r="K26" s="76"/>
     </row>
@@ -10055,7 +10054,7 @@
       <c r="I27" s="83"/>
       <c r="J27" s="85">
         <f>0.13*G26*((114907.3+6135.3)/15)</f>
-        <v>885.12401250000016</v>
+        <v>860.34054015000015</v>
       </c>
       <c r="K27" s="76"/>
     </row>
@@ -10105,23 +10104,23 @@
       </c>
       <c r="C30" s="82">
         <f>TRUNC(D31/0.15,0)</f>
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D30" s="83">
         <f>E20-0.1</f>
         <v>3.9</v>
       </c>
       <c r="E30" s="83">
-        <f>8*8/162</f>
-        <v>0.39506172839506171</v>
+        <f>10*10/162</f>
+        <v>0.61728395061728392</v>
       </c>
       <c r="F30" s="83">
         <f>PRODUCT(C30:E30)</f>
-        <v>126.34074074074074</v>
+        <v>192.59259259259258</v>
       </c>
       <c r="G30" s="83">
         <f>F30/1000</f>
-        <v>0.12634074074074075</v>
+        <v>0.19259259259259259</v>
       </c>
       <c r="H30" s="83"/>
       <c r="I30" s="83"/>
@@ -10137,7 +10136,7 @@
       </c>
       <c r="D31" s="8">
         <f>D20-0.1</f>
-        <v>12.4</v>
+        <v>12.05</v>
       </c>
       <c r="E31" s="83">
         <f>8*8/162</f>
@@ -10145,11 +10144,11 @@
       </c>
       <c r="F31" s="83">
         <f>PRODUCT(C31:E31)</f>
-        <v>127.36790123456791</v>
+        <v>123.77283950617284</v>
       </c>
       <c r="G31" s="83">
         <f>F31/1000</f>
-        <v>0.1273679012345679</v>
+        <v>0.12377283950617285</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -10169,7 +10168,7 @@
       <c r="F32" s="83"/>
       <c r="G32" s="53">
         <f>SUM(G30:G31)</f>
-        <v>0.25370864197530862</v>
+        <v>0.31636543209876544</v>
       </c>
       <c r="H32" s="53" t="s">
         <v>49</v>
@@ -10179,7 +10178,7 @@
       </c>
       <c r="J32" s="84">
         <f>G32*I32</f>
-        <v>31495.390814814811</v>
+        <v>39273.604740740739</v>
       </c>
       <c r="K32" s="76"/>
     </row>
@@ -10197,7 +10196,7 @@
       <c r="I33" s="83"/>
       <c r="J33" s="85">
         <f>0.13*G32*110960</f>
-        <v>3659.6964187654321</v>
+        <v>4563.5080849382721</v>
       </c>
       <c r="K33" s="76"/>
     </row>
@@ -10243,7 +10242,7 @@
       </c>
       <c r="D36" s="83">
         <f>D20</f>
-        <v>12.5</v>
+        <v>12.15</v>
       </c>
       <c r="E36" s="83">
         <f>E20</f>
@@ -10254,7 +10253,7 @@
       </c>
       <c r="G36" s="79">
         <f>PRODUCT(C36:F36)</f>
-        <v>7.5</v>
+        <v>7.29</v>
       </c>
       <c r="H36" s="83"/>
       <c r="I36" s="83"/>
@@ -10272,7 +10271,7 @@
       <c r="F37" s="83"/>
       <c r="G37" s="53">
         <f>SUM(G36:G36)</f>
-        <v>7.5</v>
+        <v>7.29</v>
       </c>
       <c r="H37" s="53" t="s">
         <v>49</v>
@@ -10282,7 +10281,7 @@
       </c>
       <c r="J37" s="84">
         <f>G37*I37</f>
-        <v>86911.274999999994</v>
+        <v>84477.759300000005</v>
       </c>
       <c r="K37" s="76"/>
     </row>
@@ -10300,7 +10299,7 @@
       <c r="I38" s="83"/>
       <c r="J38" s="85">
         <f>0.13*G37*((128662.2+6685.5)/15)</f>
-        <v>8797.6005000000005</v>
+        <v>8551.267686000001</v>
       </c>
       <c r="K38" s="76"/>
     </row>
@@ -10344,7 +10343,7 @@
       </c>
       <c r="D41" s="78">
         <f>D10</f>
-        <v>12.5</v>
+        <v>12.15</v>
       </c>
       <c r="E41" s="78">
         <v>0.45</v>
@@ -10355,7 +10354,7 @@
       </c>
       <c r="G41" s="79">
         <f>PRODUCT(C41:F41)</f>
-        <v>14.0625</v>
+        <v>13.668750000000001</v>
       </c>
       <c r="H41" s="80"/>
       <c r="I41" s="80"/>
@@ -10380,7 +10379,7 @@
       <c r="F42" s="83"/>
       <c r="G42" s="53">
         <f>SUM(G41:G41)</f>
-        <v>14.0625</v>
+        <v>13.668750000000001</v>
       </c>
       <c r="H42" s="53" t="s">
         <v>49</v>
@@ -10390,7 +10389,7 @@
       </c>
       <c r="J42" s="84">
         <f>G42*I42</f>
-        <v>142224.1875</v>
+        <v>138241.91025000002</v>
       </c>
       <c r="K42" s="76"/>
     </row>
@@ -10408,7 +10407,7 @@
       <c r="I43" s="83"/>
       <c r="J43" s="85">
         <f>0.13*G42*((28040.8)/5)</f>
-        <v>10252.4175</v>
+        <v>9965.3498100000015</v>
       </c>
       <c r="K43" s="76"/>
     </row>
@@ -10495,7 +10494,7 @@
       <c r="I47" s="81"/>
       <c r="J47" s="81">
         <f>SUM(J10:J45)</f>
-        <v>338168.77862108022</v>
+        <v>338380.42085432902</v>
       </c>
       <c r="K47" s="76"/>
     </row>
@@ -10519,7 +10518,7 @@
       </c>
       <c r="C49" s="137">
         <f>J47</f>
-        <v>338168.77862108022</v>
+        <v>338380.42085432902</v>
       </c>
       <c r="D49" s="137"/>
       <c r="E49" s="79">
@@ -10561,7 +10560,7 @@
       <c r="D51" s="138"/>
       <c r="E51" s="79">
         <f>C51/C49*100</f>
-        <v>84.277443104629086</v>
+        <v>84.224731230147327</v>
       </c>
       <c r="F51" s="90"/>
       <c r="G51" s="89"/>
@@ -10577,12 +10576,12 @@
       </c>
       <c r="C52" s="137">
         <f>C49-C51</f>
-        <v>53168.778621080215</v>
+        <v>53380.420854329015</v>
       </c>
       <c r="D52" s="137"/>
       <c r="E52" s="79">
         <f>100-E51</f>
-        <v>15.722556895370914</v>
+        <v>15.775268769852673</v>
       </c>
       <c r="F52" s="90"/>
       <c r="G52" s="89"/>
@@ -10702,6 +10701,13 @@
     <row r="111" s="75" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="A7:F7"/>
@@ -10710,13 +10716,6 @@
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>